<commit_message>
updated sheet for sprint1
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle9\OneDrive\Desktop\MSU-School\2019\CSC450\LeafDiskAnalyzer\LeafDiskAnalyzer\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{D16B1E28-01D3-4AC1-906D-3A0F19B52CF5}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{883207E8-07AC-4C0C-960A-DF90FF1F6485}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -299,7 +299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Sprint1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -362,11 +362,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$10:$I$10</c15:sqref>
+                    <c15:sqref>Sprint1!$B$10:$I$10</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$B$10:$H$10</c:f>
+              <c:f>Sprint1!$B$10:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -406,7 +406,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sprint1!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -469,11 +469,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$11:$I$11</c15:sqref>
+                    <c15:sqref>Sprint1!$B$11:$I$11</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$B$11:$H$11</c:f>
+              <c:f>Sprint1!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>

</xml_diff>

<commit_message>
udated Sprint1 and 2 Tables and Burndown charts
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle9\OneDrive\Desktop\MSU-School\2019\CSC450\LeafDiskAnalyzer\LeafDiskAnalyzer\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b9050db097f4435/Desktop/MSU-School/2019/CSC450/LeafDiskAnalyzer/LeafDiskAnalyzer/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{883207E8-07AC-4C0C-960A-DF90FF1F6485}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{C1BAD3C7-B5CC-4DA1-A422-D5E07A3164E1}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="28">
   <si>
     <t>Task #</t>
   </si>
@@ -90,37 +91,31 @@
     <t>N/A</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Author: Kyle Sargent</t>
   </si>
   <si>
     <t>Last Updated</t>
   </si>
   <si>
-    <t>US01-T02</t>
+    <t>US001-T01</t>
   </si>
   <si>
-    <t>US01-T01</t>
+    <t>US001-T03</t>
   </si>
   <si>
-    <t>US02-T01</t>
+    <t>US003-T01</t>
   </si>
   <si>
-    <t>US02-T02</t>
+    <t>US004-T01</t>
   </si>
   <si>
-    <t>US03-T01</t>
+    <t>US004-T02</t>
   </si>
   <si>
-    <t>US03-T02</t>
+    <t>US005-T01</t>
   </si>
   <si>
-    <t>US04-T01</t>
-  </si>
-  <si>
-    <t>US04-T02</t>
+    <t>No Tasks Completed During Sprint 1. Sprint 1 was our planning sprint, thus any "completed tasks"</t>
   </si>
 </sst>
 </file>
@@ -240,7 +235,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint 1- Burndown Chart (7 days in)</a:t>
+              <a:t>Sprint 1- Burndown Chart </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -249,8 +244,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19422900262467191"/>
-          <c:y val="3.2407407407407406E-2"/>
+          <c:x val="0.28173895476669236"/>
+          <c:y val="4.6296296296296294E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -370,27 +365,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -477,25 +451,593 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-179E-4A82-A9F9-58A06EC760A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="597292848"/>
+        <c:axId val="597295144"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="597292848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="597295144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="597295144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="597292848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 2-Burndown Chart (7 days in)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19422900262467191"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint2!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>Actual Hours Remaining</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>14</c:v>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sprint2!$B$10:$I$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sprint2!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-62C3-4942-80BE-EB2757895BB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint2!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Hours Remaining</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sprint2!$B$11:$I$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sprint2!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -504,7 +1046,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-179E-4A82-A9F9-58A06EC760A6}"/>
+              <c16:uniqueId val="{00000001-62C3-4942-80BE-EB2757895BB6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -861,6 +1403,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -1357,7 +1936,544 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCD79A4-CE69-4152-AE25-F9F7F7CBA406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1374,14 +2490,16 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCD79A4-CE69-4152-AE25-F9F7F7CBA406}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6549BEE0-C818-437E-896B-727411047DAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1418,6 +2536,31 @@
     <tableColumn id="14" xr3:uid="{2254270C-B57E-4814-A853-300CAEE1A916}" name=" Day 12"/>
     <tableColumn id="15" xr3:uid="{989FE709-8841-43BA-BFAA-3398FB879B32}" name=" Day 13"/>
     <tableColumn id="16" xr3:uid="{0658BE80-132A-4E31-B365-25A718A1FBCE}" name=" Day 14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70FCEFFC-3AB9-4275-96D5-32408D22FAEA}" name="Table13" displayName="Table13" ref="A1:P11" totalsRowShown="0">
+  <autoFilter ref="A1:P11" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{564E2E6B-FB07-4A96-A999-7DF82171EC04}" name="Task #"/>
+    <tableColumn id="2" xr3:uid="{8D94BA0C-0FA9-4D99-ACB1-E733AAED9C46}" name="Hours Needed"/>
+    <tableColumn id="3" xr3:uid="{B48BA6CE-38CA-4134-B5B0-ED5396971B39}" name="Day 1"/>
+    <tableColumn id="4" xr3:uid="{CE069B49-0967-42CC-A8E4-73AF4A266141}" name=" Day 2"/>
+    <tableColumn id="5" xr3:uid="{FA263AEF-458D-4D84-AACD-9DF9684ACB3A}" name="Day 3"/>
+    <tableColumn id="6" xr3:uid="{130B550F-9BF2-44A1-8ABC-3D618F03A288}" name=" Day 4"/>
+    <tableColumn id="7" xr3:uid="{F703691B-183B-4C00-9182-D9E792FA1066}" name=" Day 5"/>
+    <tableColumn id="8" xr3:uid="{C19B2DC5-1A8D-436C-86E4-F428ECDCF842}" name=" Day 6"/>
+    <tableColumn id="9" xr3:uid="{70A0F4F5-4A6C-40F9-91E0-36152E65E103}" name=" Day 7"/>
+    <tableColumn id="10" xr3:uid="{7374A8AD-D13F-4A70-BA0B-9F1A89F5C18E}" name=" Day 8"/>
+    <tableColumn id="11" xr3:uid="{6E1EA008-3FC9-457C-BE6E-91A62DAFD5EF}" name=" Day 9"/>
+    <tableColumn id="12" xr3:uid="{F008105B-31DE-452E-8D2B-8FC62AE934B4}" name=" Day 10"/>
+    <tableColumn id="13" xr3:uid="{C0700E9A-111B-4EA9-8D44-560B63ED19C6}" name=" Day 11"/>
+    <tableColumn id="14" xr3:uid="{ABED520C-EAE7-4FB3-B527-514ECFA9568C}" name=" Day 12"/>
+    <tableColumn id="15" xr3:uid="{1F8F4BFE-6799-467F-A73E-2CA7F32DD689}" name=" Day 13"/>
+    <tableColumn id="16" xr3:uid="{AD9D548F-60BC-4D2B-950E-3099930CB906}" name=" Day 14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1723,7 +2866,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1785,31 +2928,565 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="3">
+        <f ca="1">TODAY()-9</f>
+        <v>43507</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
+  <dimension ref="A1:P34"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -1829,8 +3506,8 @@
       <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="P2">
-        <v>0</v>
+      <c r="P2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1840,26 +3517,26 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1879,37 +3556,37 @@
       <c r="O3" t="s">
         <v>18</v>
       </c>
-      <c r="P3">
-        <v>0</v>
+      <c r="P3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1929,37 +3606,37 @@
       <c r="O4" t="s">
         <v>18</v>
       </c>
-      <c r="P4">
-        <v>0</v>
+      <c r="P4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -1979,37 +3656,37 @@
       <c r="O5" t="s">
         <v>18</v>
       </c>
-      <c r="P5">
-        <v>0</v>
+      <c r="P5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -2029,37 +3706,37 @@
       <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="P6">
-        <v>0</v>
+      <c r="P6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -2079,108 +3756,8 @@
       <c r="O7" t="s">
         <v>18</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
+      <c r="P7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -2188,122 +3765,58 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <f>SUM(B2:B9)</f>
-        <v>15</v>
-      </c>
-      <c r="C10" s="1">
-        <f>B10-SUM(C2:C9)</f>
-        <v>13</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" ref="D10:I10" si="0">C10-SUM(D2:D9)</f>
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
+        <f>SUM(B2:B7)</f>
+        <v>6.5</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <f>SUM(B2:B9)</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="2">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2">
-        <v>8</v>
-      </c>
-      <c r="H11" s="2">
         <v>7</v>
       </c>
-      <c r="I11" s="2">
-        <v>6</v>
-      </c>
-      <c r="J11" s="2">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2">
-        <v>4</v>
-      </c>
-      <c r="L11" s="2">
-        <v>3</v>
-      </c>
-      <c r="M11" s="2">
-        <v>2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="3">
         <f ca="1">TODAY()</f>
-        <v>43507</v>
+        <v>43516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Sprint1 and 2 Tables and Burndown charts
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b9050db097f4435/Desktop/MSU-School/2019/CSC450/LeafDiskAnalyzer/LeafDiskAnalyzer/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{C1BAD3C7-B5CC-4DA1-A422-D5E07A3164E1}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{733E55F6-B330-4D94-9B09-73DE2BE41849}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="28">
   <si>
     <t>Task #</t>
   </si>
@@ -2865,8 +2865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDA324-FDEE-4514-95CB-47D5679C2716}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3399,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,6 +3757,106 @@
         <v>18</v>
       </c>
       <c r="P7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated Sprint2 Burndown Chart/Graph, subject to change
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b9050db097f4435/Desktop/MSU-School/2019/CSC450/LeafDiskAnalyzer/LeafDiskAnalyzer/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{733E55F6-B330-4D94-9B09-73DE2BE41849}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{DEE25762-FBFB-407F-A08F-ACB2FE816517}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="36">
   <si>
     <t>Task #</t>
   </si>
@@ -106,16 +106,40 @@
     <t>US003-T01</t>
   </si>
   <si>
-    <t>US004-T01</t>
+    <t>No Tasks Completed During Sprint 1. Sprint 1 was our planning sprint, thus any "completed tasks"</t>
   </si>
   <si>
-    <t>US004-T02</t>
+    <t>US001-T02</t>
   </si>
   <si>
-    <t>US005-T01</t>
+    <t>US001-T04</t>
   </si>
   <si>
-    <t>No Tasks Completed During Sprint 1. Sprint 1 was our planning sprint, thus any "completed tasks"</t>
+    <t>US001-T05</t>
+  </si>
+  <si>
+    <t>US001-T06</t>
+  </si>
+  <si>
+    <t>US003-T02</t>
+  </si>
+  <si>
+    <t>US003-T04</t>
+  </si>
+  <si>
+    <t>US003-T03</t>
+  </si>
+  <si>
+    <t>US001-T07</t>
+  </si>
+  <si>
+    <t>US001-T08</t>
+  </si>
+  <si>
+    <t>Estimated Hours Needed</t>
+  </si>
+  <si>
+    <t>Last Edited By: Kyle Sargent</t>
   </si>
 </sst>
 </file>
@@ -818,19 +842,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint 2-Burndown Chart (7 days in)</a:t>
+              <a:t>Sprint 2- Burndown</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.19422900262467191"/>
-          <c:y val="3.2407407407407406E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -877,7 +898,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$A$10</c:f>
+              <c:f>Sprint2!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -906,7 +927,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="7"/>
+              <c:ptCount val="13"/>
               <c:pt idx="0">
                 <c:v>1</c:v>
               </c:pt>
@@ -928,6 +949,24 @@
               <c:pt idx="6">
                 <c:v>7</c:v>
               </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:autoCat val="1"/>
@@ -940,16 +979,52 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sprint2!$B$10:$I$10</c15:sqref>
+                    <c15:sqref>Sprint2!$C$14:$P$14</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sprint2!$B$10:$H$10</c:f>
+              <c:f>(Sprint2!$C$14:$N$14,Sprint2!$P$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,7 +1032,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-62C3-4942-80BE-EB2757895BB6}"/>
+              <c16:uniqueId val="{00000017-E602-487D-A430-2F5CE3A6702D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -966,7 +1041,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$A$11</c:f>
+              <c:f>Sprint2!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -995,7 +1070,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="7"/>
+              <c:ptCount val="13"/>
               <c:pt idx="0">
                 <c:v>1</c:v>
               </c:pt>
@@ -1017,6 +1092,24 @@
               <c:pt idx="6">
                 <c:v>7</c:v>
               </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:autoCat val="1"/>
@@ -1029,16 +1122,52 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sprint2!$B$11:$I$11</c15:sqref>
+                    <c15:sqref>Sprint2!$C$15:$P$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sprint2!$B$11:$H$11</c:f>
+              <c:f>(Sprint2!$C$15:$N$15,Sprint2!$P$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1046,7 +1175,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-62C3-4942-80BE-EB2757895BB6}"/>
+              <c16:uniqueId val="{00000018-E602-487D-A430-2F5CE3A6702D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1059,11 +1188,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="597292848"/>
-        <c:axId val="597295144"/>
+        <c:axId val="781797536"/>
+        <c:axId val="781795896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597292848"/>
+        <c:axId val="781797536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1251,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1158,7 +1287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597295144"/>
+        <c:crossAx val="781795896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1166,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597295144"/>
+        <c:axId val="781795896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1335,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Total Hours</a:t>
+                  <a:t>Hours Worked </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1269,7 +1398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597292848"/>
+        <c:crossAx val="781797536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1404,10 +1533,13 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2478,14 +2610,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2493,13 +2625,11 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6549BEE0-C818-437E-896B-727411047DAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF68EDB7-3B0E-4447-982B-E4E957B5E6F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2542,11 +2672,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70FCEFFC-3AB9-4275-96D5-32408D22FAEA}" name="Table13" displayName="Table13" ref="A1:P11" totalsRowShown="0">
-  <autoFilter ref="A1:P11" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70FCEFFC-3AB9-4275-96D5-32408D22FAEA}" name="Table13" displayName="Table13" ref="A1:P15" totalsRowShown="0">
+  <autoFilter ref="A1:P15" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{564E2E6B-FB07-4A96-A999-7DF82171EC04}" name="Task #"/>
-    <tableColumn id="2" xr3:uid="{8D94BA0C-0FA9-4D99-ACB1-E733AAED9C46}" name="Hours Needed"/>
+    <tableColumn id="2" xr3:uid="{8D94BA0C-0FA9-4D99-ACB1-E733AAED9C46}" name="Estimated Hours Needed"/>
     <tableColumn id="3" xr3:uid="{B48BA6CE-38CA-4134-B5B0-ED5396971B39}" name="Day 1"/>
     <tableColumn id="4" xr3:uid="{CE069B49-0967-42CC-A8E4-73AF4A266141}" name=" Day 2"/>
     <tableColumn id="5" xr3:uid="{FA263AEF-458D-4D84-AACD-9DF9684ACB3A}" name="Day 3"/>
@@ -2865,8 +2995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDA324-FDEE-4514-95CB-47D5679C2716}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3368,7 +3498,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3381,8 +3511,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="3">
-        <f ca="1">TODAY()-9</f>
-        <v>43507</v>
+        <v>43508</v>
       </c>
     </row>
   </sheetData>
@@ -3397,16 +3526,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:P9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3415,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3465,458 +3594,727 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>18</v>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>18</v>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>18</v>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1">
-        <f>SUM(B2:B7)</f>
-        <v>6.5</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <f>SUM(B2:B13)</f>
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14-SUM(C2:C13)</f>
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <f>C14-SUM(D2:D13)</f>
+        <v>18</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14-SUM(E2:E13)</f>
+        <v>18</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14-SUM(F2:F13)</f>
+        <v>16</v>
+      </c>
+      <c r="G14" s="1">
+        <f>F14-SUM(G2:G13)</f>
+        <v>16</v>
+      </c>
+      <c r="H14" s="1">
+        <f>G14-SUM(H2:H13)</f>
+        <v>14</v>
+      </c>
+      <c r="I14" s="1">
+        <f>H14-SUM(I2:I13)</f>
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
+        <f>I14-SUM(J2:J13)</f>
+        <v>10</v>
+      </c>
+      <c r="K14" s="1">
+        <f>Table13[[#This Row],[ Day 8]]-SUM(K2:K13)</f>
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f>Table13[[#This Row],[ Day 9]]-SUM(L2:L13)</f>
+        <v>4</v>
+      </c>
+      <c r="M14" s="1">
+        <f>Table13[[#This Row],[ Day 10]]-SUM(M2:M13)</f>
+        <v>3</v>
+      </c>
+      <c r="N14" s="1">
+        <f>Table13[[#This Row],[ Day 11]]-SUM(N2:N13)</f>
+        <v>2</v>
+      </c>
+      <c r="O14" s="1">
+        <f>Table13[[#This Row],[ Day 12]]-SUM(O2:O13)</f>
+        <v>1</v>
+      </c>
+      <c r="P14" s="1">
+        <f>Table13[[#This Row],[ Day 13]]-SUM(P2:P13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="B15" s="2">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2">
+        <v>12</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
+        <v>9</v>
+      </c>
+      <c r="K15" s="2">
+        <v>8</v>
+      </c>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>19</v>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="3">
-        <f ca="1">TODAY()</f>
-        <v>43516</v>
+      <c r="B38" s="3">
+        <v>43526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated sprint2 burndown chart, velocity, and percentage complete charts
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b9050db097f4435/Desktop/MSU-School/2019/CSC450/LeafDiskAnalyzer/LeafDiskAnalyzer/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{DEE25762-FBFB-407F-A08F-ACB2FE816517}"/>
+  <xr:revisionPtr revIDLastSave="818" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FD1E7B19-9DB0-404B-B7BA-C059A3A7F6E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
+    <sheet name="Velocity" sheetId="3" r:id="rId3"/>
+    <sheet name="Percentage Complete" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="54">
   <si>
     <t>Task #</t>
   </si>
@@ -97,49 +99,103 @@
     <t>Last Updated</t>
   </si>
   <si>
-    <t>US001-T01</t>
-  </si>
-  <si>
-    <t>US001-T03</t>
-  </si>
-  <si>
-    <t>US003-T01</t>
-  </si>
-  <si>
     <t>No Tasks Completed During Sprint 1. Sprint 1 was our planning sprint, thus any "completed tasks"</t>
-  </si>
-  <si>
-    <t>US001-T02</t>
-  </si>
-  <si>
-    <t>US001-T04</t>
-  </si>
-  <si>
-    <t>US001-T05</t>
-  </si>
-  <si>
-    <t>US001-T06</t>
-  </si>
-  <si>
-    <t>US003-T02</t>
-  </si>
-  <si>
-    <t>US003-T04</t>
-  </si>
-  <si>
-    <t>US003-T03</t>
-  </si>
-  <si>
-    <t>US001-T07</t>
-  </si>
-  <si>
-    <t>US001-T08</t>
   </si>
   <si>
     <t>Estimated Hours Needed</t>
   </si>
   <si>
     <t>Last Edited By: Kyle Sargent</t>
+  </si>
+  <si>
+    <t>US003-T7</t>
+  </si>
+  <si>
+    <t>US003-T6</t>
+  </si>
+  <si>
+    <t>US003-T5</t>
+  </si>
+  <si>
+    <t>US003-T4</t>
+  </si>
+  <si>
+    <t>US003-T3</t>
+  </si>
+  <si>
+    <t>US003-T2</t>
+  </si>
+  <si>
+    <t>US003-T1</t>
+  </si>
+  <si>
+    <t>US001-T8</t>
+  </si>
+  <si>
+    <t>US001-T7</t>
+  </si>
+  <si>
+    <t>US001-T6</t>
+  </si>
+  <si>
+    <t>US001-T5</t>
+  </si>
+  <si>
+    <t>US001-T4</t>
+  </si>
+  <si>
+    <t>US001-T3</t>
+  </si>
+  <si>
+    <t>US001-T2</t>
+  </si>
+  <si>
+    <t>US001-T1</t>
+  </si>
+  <si>
+    <t>US005-T1</t>
+  </si>
+  <si>
+    <t>Sprint #</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>US001</t>
+  </si>
+  <si>
+    <t>US002</t>
+  </si>
+  <si>
+    <t>US003</t>
+  </si>
+  <si>
+    <t>US004</t>
+  </si>
+  <si>
+    <t>US005</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Total Percent Complete</t>
+  </si>
+  <si>
+    <t>Last Updated By: Kyle Sargent</t>
+  </si>
+  <si>
+    <t>Last Update On: 3/3/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Update On: 3/3/19 </t>
   </si>
 </sst>
 </file>
@@ -194,11 +250,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -898,7 +958,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$A$14</c:f>
+              <c:f>Sprint2!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -979,52 +1039,52 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sprint2!$C$14:$P$14</c15:sqref>
+                    <c15:sqref>Sprint2!$C$18:$P$18</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sprint2!$C$14:$N$14,Sprint2!$P$14)</c:f>
+              <c:f>(Sprint2!$C$18:$N$18,Sprint2!$P$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,7 +1101,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$A$15</c:f>
+              <c:f>Sprint2!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1122,19 +1182,19 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sprint2!$C$15:$P$15</c15:sqref>
+                    <c15:sqref>Sprint2!$C$19:$P$19</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sprint2!$C$15:$N$15,Sprint2!$P$15)</c:f>
+              <c:f>(Sprint2!$C$19:$N$19,Sprint2!$P$19)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
@@ -1143,22 +1203,22 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
@@ -1495,6 +1555,1231 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 2 Velocity Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Velocity!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Velocity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Velocity!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DD4A-4ECA-B1B5-844E20FF27C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="756536992"/>
+        <c:axId val="756537320"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Velocity!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Sprint #</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent2">
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent2">
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="85000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:lumMod val="95000"/>
+                                <a:alpha val="54000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Velocity!$A$2:$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-DD4A-4ECA-B1B5-844E20FF27C0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="756536992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sprint Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="756537320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="756537320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Velocity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="756536992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent Complete - Per User Story</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5160104986876636E-2"/>
+          <c:y val="0.22666375036453776"/>
+          <c:w val="0.70335586176727904"/>
+          <c:h val="0.66745953630796151"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Percentage Complete'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percent Complete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-401D-41B6-872A-3A0B4A3E08E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-401D-41B6-872A-3A0B4A3E08E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-401D-41B6-872A-3A0B4A3E08E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-401D-41B6-872A-3A0B4A3E08E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.77752624671916E-2"/>
+                  <c:y val="-4.2133275007290756E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-401D-41B6-872A-3A0B4A3E08E6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Percentage Complete'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>US001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>US002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>US003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>US004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>US005</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Percentage Complete'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-401D-41B6-872A-3A0B4A3E08E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -1572,6 +2857,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -2096,6 +3461,998 @@
           <a:schemeClr val="lt1">
             <a:lumMod val="95000"/>
             <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2609,16 +4966,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1400735</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>8740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:colOff>271182</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>8741</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2626,6 +4983,88 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF68EDB7-3B0E-4447-982B-E4E957B5E6F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4994936F-3B85-480E-8636-7AEE09F7D1BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5368BFE1-B07E-4947-B8A4-42BF727139EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2672,8 +5111,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70FCEFFC-3AB9-4275-96D5-32408D22FAEA}" name="Table13" displayName="Table13" ref="A1:P15" totalsRowShown="0">
-  <autoFilter ref="A1:P15" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70FCEFFC-3AB9-4275-96D5-32408D22FAEA}" name="Table13" displayName="Table13" ref="A1:P19" totalsRowShown="0">
+  <autoFilter ref="A1:P19" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{564E2E6B-FB07-4A96-A999-7DF82171EC04}" name="Task #"/>
     <tableColumn id="2" xr3:uid="{8D94BA0C-0FA9-4D99-ACB1-E733AAED9C46}" name="Estimated Hours Needed"/>
@@ -2996,7 +5435,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3497,9 +5936,13 @@
       <c r="P11" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -3512,6 +5955,1012 @@
       </c>
       <c r="B34" s="3">
         <v>43508</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
+  <dimension ref="A1:P42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0.5</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <f>SUM(B2:B17)</f>
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <f>B18-SUM(C2:C13)</f>
+        <v>22</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" ref="D18:P18" si="0">C18-SUM(D2:D13)</f>
+        <v>21</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2">
+        <v>14</v>
+      </c>
+      <c r="G19" s="2">
+        <v>12</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2">
+        <v>9</v>
+      </c>
+      <c r="J19" s="2">
+        <v>8</v>
+      </c>
+      <c r="K19" s="2">
+        <v>6</v>
+      </c>
+      <c r="L19" s="2">
+        <v>4</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3</v>
+      </c>
+      <c r="N19" s="2">
+        <v>2</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="3">
+        <v>43527</v>
       </c>
     </row>
   </sheetData>
@@ -3524,805 +6973,180 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
-  <dimension ref="A1:P38"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1084ABB9-FA7C-4FCD-BBA0-C718156B219C}">
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B3">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
+      <c r="C3">
+        <v>3.5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <f>SUM(B2:B13)</f>
-        <v>19</v>
-      </c>
-      <c r="C14" s="1">
-        <f>B14-SUM(C2:C13)</f>
-        <v>19</v>
-      </c>
-      <c r="D14" s="1">
-        <f>C14-SUM(D2:D13)</f>
-        <v>18</v>
-      </c>
-      <c r="E14" s="1">
-        <f>D14-SUM(E2:E13)</f>
-        <v>18</v>
-      </c>
-      <c r="F14" s="1">
-        <f>E14-SUM(F2:F13)</f>
-        <v>16</v>
-      </c>
-      <c r="G14" s="1">
-        <f>F14-SUM(G2:G13)</f>
-        <v>16</v>
-      </c>
-      <c r="H14" s="1">
-        <f>G14-SUM(H2:H13)</f>
-        <v>14</v>
-      </c>
-      <c r="I14" s="1">
-        <f>H14-SUM(I2:I13)</f>
-        <v>10</v>
-      </c>
-      <c r="J14" s="1">
-        <f>I14-SUM(J2:J13)</f>
-        <v>10</v>
-      </c>
-      <c r="K14" s="1">
-        <f>Table13[[#This Row],[ Day 8]]-SUM(K2:K13)</f>
-        <v>8</v>
-      </c>
-      <c r="L14" s="1">
-        <f>Table13[[#This Row],[ Day 9]]-SUM(L2:L13)</f>
-        <v>4</v>
-      </c>
-      <c r="M14" s="1">
-        <f>Table13[[#This Row],[ Day 10]]-SUM(M2:M13)</f>
-        <v>3</v>
-      </c>
-      <c r="N14" s="1">
-        <f>Table13[[#This Row],[ Day 11]]-SUM(N2:N13)</f>
-        <v>2</v>
-      </c>
-      <c r="O14" s="1">
-        <f>Table13[[#This Row],[ Day 12]]-SUM(O2:O13)</f>
-        <v>1</v>
-      </c>
-      <c r="P14" s="1">
-        <f>Table13[[#This Row],[ Day 13]]-SUM(P2:P13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2">
-        <v>17</v>
-      </c>
-      <c r="E15" s="2">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2">
-        <v>14</v>
-      </c>
-      <c r="G15" s="2">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2">
-        <v>12</v>
-      </c>
-      <c r="I15" s="2">
-        <v>10</v>
-      </c>
-      <c r="J15" s="2">
-        <v>9</v>
-      </c>
-      <c r="K15" s="2">
-        <v>8</v>
-      </c>
-      <c r="L15" s="2">
-        <v>5</v>
-      </c>
-      <c r="M15" s="2">
-        <v>3</v>
-      </c>
-      <c r="N15" s="2">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2">
-        <v>1</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="3">
-        <v>43526</v>
-      </c>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877D0DD0-5ABF-4A89-80A6-BA23EEBC79DF}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="C2" s="4">
+        <f>IF(B2=100%, 100/5, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C6" si="0">IF(B3=100%, 100/5, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated sprint burndown for sprint 3 and uploading S3 Retrospect
</commit_message>
<xml_diff>
--- a/documents/Sprint-Burndown.xlsx
+++ b/documents/Sprint-Burndown.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b9050db097f4435/Desktop/MSU-School/2019/CSC450/LeafDiskAnalyzer/LeafDiskAnalyzer/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="818" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FD1E7B19-9DB0-404B-B7BA-C059A3A7F6E8}"/>
+  <xr:revisionPtr revIDLastSave="1368" documentId="8_{E1A5174E-C441-4E63-B308-0CECCD812201}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{7970026A-2FB5-4199-927C-E0B94F0E6FFB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
+    <workbookView xWindow="14280" yWindow="240" windowWidth="17280" windowHeight="9420" firstSheet="2" activeTab="2" xr2:uid="{735C6AD7-B7C0-4B82-B1FC-BDA75AEFB7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
-    <sheet name="Velocity" sheetId="3" r:id="rId3"/>
-    <sheet name="Percentage Complete" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint3" sheetId="5" r:id="rId3"/>
+    <sheet name="Velocity" sheetId="3" r:id="rId4"/>
+    <sheet name="Percentage Complete" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="81">
   <si>
     <t>Task #</t>
   </si>
@@ -192,16 +193,100 @@
     <t>Last Updated By: Kyle Sargent</t>
   </si>
   <si>
-    <t>Last Update On: 3/3/19</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Last Update On: 3/3/19 </t>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>US001-T9</t>
+  </si>
+  <si>
+    <t>US001-T10</t>
+  </si>
+  <si>
+    <t>US005-T2</t>
+  </si>
+  <si>
+    <t>US005-T3</t>
+  </si>
+  <si>
+    <t>US005-T4</t>
+  </si>
+  <si>
+    <t>US005-T5</t>
+  </si>
+  <si>
+    <t>US005-T6</t>
+  </si>
+  <si>
+    <t>US005-T7</t>
+  </si>
+  <si>
+    <t>US005-T8</t>
+  </si>
+  <si>
+    <t>US005-T9</t>
+  </si>
+  <si>
+    <t>US005-T10</t>
+  </si>
+  <si>
+    <t>US005-T11</t>
+  </si>
+  <si>
+    <t>US005-T12</t>
+  </si>
+  <si>
+    <t>US005-T13</t>
+  </si>
+  <si>
+    <t>US005-T14</t>
+  </si>
+  <si>
+    <t>US004-T1</t>
+  </si>
+  <si>
+    <t>US004-T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Update On: 3/15/19 </t>
+  </si>
+  <si>
+    <t>US005-T15</t>
+  </si>
+  <si>
+    <t>US005-T16</t>
+  </si>
+  <si>
+    <t>US004-T3</t>
+  </si>
+  <si>
+    <t>US004-T4</t>
+  </si>
+  <si>
+    <t>US004-T5</t>
+  </si>
+  <si>
+    <t>Last Update On: 3/24/19</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,12 +335,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1596,7 +1682,701 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint 2 Velocity Chart</a:t>
+              <a:t>Sprint 3- Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint3!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Hours Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="13"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sprint3!$C$26:$P$26</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sprint3!$C$26:$N$26,Sprint3!$P$26)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AEF-49A1-80B8-BCA71ACFD0B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint3!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Hours Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="13"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sprint3!$C$27:$P$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sprint3!$C$27:$N$27,Sprint3!$P$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2AEF-49A1-80B8-BCA71ACFD0B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="781797536"/>
+        <c:axId val="781795896"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="781797536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="781795896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="781795896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hours Worked </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="781797536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocity Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1752,17 +2532,37 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Velocity!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>S1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Velocity!$C$2:$C$3</c:f>
+              <c:f>Velocity!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0">
+                  <c:v>4.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,6 +2704,29 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Velocity!$A$2:$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>S1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>S2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>S3</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
@@ -1917,10 +2740,10 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>1</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2209,7 +3032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2400,6 +3223,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-849D-406F-A431-4E1C0D2F0C36}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2653,7 +3481,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.78</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2937,6 +3765,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -3930,7 +4798,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3952,11 +4820,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
             <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4033,7 +4901,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -4043,7 +4911,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -4053,7 +4921,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -4073,7 +4941,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -4092,7 +4960,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4129,7 +4997,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4153,7 +5021,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -4172,7 +5040,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4190,7 +5058,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -4198,7 +5066,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4217,7 +5085,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
@@ -4235,7 +5103,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -4254,7 +5122,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -4283,7 +5151,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -4291,7 +5159,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4361,7 +5229,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -4387,7 +5255,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4419,13 +5287,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5007,6 +6371,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>547295</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>168760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>240702</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>168761</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E489EC11-24C8-4868-A11C-CB89B89CE067}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -5044,20 +6451,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1386840</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5130,6 +6537,31 @@
     <tableColumn id="14" xr3:uid="{ABED520C-EAE7-4FB3-B527-514ECFA9568C}" name=" Day 12"/>
     <tableColumn id="15" xr3:uid="{1F8F4BFE-6799-467F-A73E-2CA7F32DD689}" name=" Day 13"/>
     <tableColumn id="16" xr3:uid="{AD9D548F-60BC-4D2B-950E-3099930CB906}" name=" Day 14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4750CAA5-070E-477D-A21F-D8AE215EACEC}" name="Table134" displayName="Table134" ref="A1:P27" totalsRowShown="0">
+  <autoFilter ref="A1:P27" xr:uid="{28027A2F-D878-4CBF-9E7F-76A985DA3A5A}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{BB5E001F-ADD5-4720-9B59-4C384987525C}" name="Task #"/>
+    <tableColumn id="2" xr3:uid="{3E44C472-0823-42B4-A1FF-589EF5EB6576}" name="Estimated Hours Needed"/>
+    <tableColumn id="3" xr3:uid="{A0A371B3-9899-4DD3-BA22-BB185917FA31}" name="Day 1"/>
+    <tableColumn id="4" xr3:uid="{78BA5753-CA0D-41FC-9088-0EAA63C20969}" name=" Day 2"/>
+    <tableColumn id="5" xr3:uid="{0E603078-A559-489C-8036-DCD668D6E561}" name="Day 3"/>
+    <tableColumn id="6" xr3:uid="{D17E6C85-C9C9-4502-8A52-768B1E62AC29}" name=" Day 4"/>
+    <tableColumn id="7" xr3:uid="{827BE21D-458A-4371-949D-3983B8BB6FCF}" name=" Day 5"/>
+    <tableColumn id="8" xr3:uid="{5A831925-B37D-463C-83E9-95B31B067AAF}" name=" Day 6"/>
+    <tableColumn id="9" xr3:uid="{EC9DAC7D-FCD0-4AE9-8FEE-4035D595C292}" name=" Day 7"/>
+    <tableColumn id="10" xr3:uid="{81E6B48C-59A5-441F-B2BB-E23DBC7A5DF7}" name=" Day 8"/>
+    <tableColumn id="11" xr3:uid="{6C23641E-791A-43BA-8EF9-47E52852A6FD}" name=" Day 9"/>
+    <tableColumn id="12" xr3:uid="{076B70CC-D9EB-418C-B96E-FB3BC194D123}" name=" Day 10"/>
+    <tableColumn id="13" xr3:uid="{33DD3C3D-1316-454B-99A5-3015EA94E30F}" name=" Day 11"/>
+    <tableColumn id="14" xr3:uid="{472B9F04-E86E-4480-A614-CED3BCE2B0CB}" name=" Day 12"/>
+    <tableColumn id="15" xr3:uid="{5E323CC0-86B2-4920-A71C-6AF52E1051FF}" name=" Day 13"/>
+    <tableColumn id="16" xr3:uid="{4F382D7A-F9C3-434E-9256-EC5B30EBCE97}" name=" Day 14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5936,13 +7368,13 @@
       <c r="P11" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -5974,7 +7406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EECDD8-AA1C-4183-90FC-03AD09FA0303}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -6974,11 +8406,1414 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0F916C-DE26-4A19-AA85-50E5F724E128}">
+  <dimension ref="A1:P50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.25</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.25</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.5</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.5</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>80</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
+        <f>SUM(B2:B25)</f>
+        <v>32</v>
+      </c>
+      <c r="C26" s="1">
+        <f>Table134[[#This Row],[Estimated Hours Needed]]-SUM(C2:C24)</f>
+        <v>29</v>
+      </c>
+      <c r="D26" s="1">
+        <f>Table134[[#This Row],[Day 1]]-SUM(D2:D24)</f>
+        <v>27.75</v>
+      </c>
+      <c r="E26" s="1">
+        <f>Table134[[#This Row],[ Day 2]]-SUM(E2:E24)</f>
+        <v>26.75</v>
+      </c>
+      <c r="F26" s="1">
+        <f>Table134[[#This Row],[Day 3]]-SUM(F2:F24)</f>
+        <v>26.25</v>
+      </c>
+      <c r="G26" s="1">
+        <f>Table134[[#This Row],[ Day 4]]-SUM(G2:G24)</f>
+        <v>26.25</v>
+      </c>
+      <c r="H26" s="1">
+        <f>Table134[[#This Row],[ Day 5]]-SUM(H2:H24)</f>
+        <v>24.75</v>
+      </c>
+      <c r="I26" s="1">
+        <f>Table134[[#This Row],[ Day 6]]-SUM(I2:I24)</f>
+        <v>23.25</v>
+      </c>
+      <c r="J26" s="1">
+        <f>Table134[[#This Row],[ Day 7]]-SUM(J2:J24)</f>
+        <v>22</v>
+      </c>
+      <c r="K26" s="1">
+        <f>Table134[[#This Row],[ Day 8]]-SUM(K2:K24)</f>
+        <v>21.5</v>
+      </c>
+      <c r="L26" s="1">
+        <f>Table134[[#This Row],[ Day 9]]-SUM(L2:L24)</f>
+        <v>11</v>
+      </c>
+      <c r="M26" s="1">
+        <f>Table134[[#This Row],[ Day 10]]-SUM(M2:M24)</f>
+        <v>10</v>
+      </c>
+      <c r="N26" s="1">
+        <f>Table134[[#This Row],[ Day 11]]-SUM(N2:N24)</f>
+        <v>8</v>
+      </c>
+      <c r="O26" s="1">
+        <f>Table134[[#This Row],[ Day 12]]-SUM(O2:O24)</f>
+        <v>7</v>
+      </c>
+      <c r="P26" s="1">
+        <f>Table134[[#This Row],[ Day 13]]-SUM(P2:P24)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2">
+        <f>SUM(B2:B25)</f>
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2">
+        <v>24</v>
+      </c>
+      <c r="E27" s="2">
+        <v>22</v>
+      </c>
+      <c r="F27" s="2">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2">
+        <v>18</v>
+      </c>
+      <c r="H27" s="2">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2">
+        <v>14</v>
+      </c>
+      <c r="J27" s="2">
+        <v>11</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9</v>
+      </c>
+      <c r="L27" s="2">
+        <v>7</v>
+      </c>
+      <c r="M27" s="2">
+        <v>5</v>
+      </c>
+      <c r="N27" s="2">
+        <v>4</v>
+      </c>
+      <c r="O27" s="2">
+        <v>2</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="3">
+        <v>43548</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1084ABB9-FA7C-4FCD-BBA0-C718156B219C}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6998,8 +9833,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>53</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -7009,29 +9844,42 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>54</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
       <c r="C3">
+        <f>B3/2</f>
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5">
+        <f>B4/3</f>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7043,12 +9891,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877D0DD0-5ABF-4A89-80A6-BA23EEBC79DF}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7073,11 +9921,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="4">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4">
-        <f>IF(B2=100%, 100/5, 0)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7128,18 +9975,18 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>